<commit_message>
Agrega excel calculo largos muro
</commit_message>
<xml_diff>
--- a/Tarea 02/Espesores losas.xlsx
+++ b/Tarea 02/Espesores losas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Google Drive\Trabajos\Proyecto de Hormigón Armado\proyecto-CI5206\Tarea 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{65D0CDB1-BBDF-40F1-9793-4D2786D008C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{776EBD55-6951-4FEF-AC4F-7B17FD5359B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{64A3EC0E-03C2-45A2-90E2-B3D1165799B2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>Losa</t>
   </si>
@@ -92,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -104,6 +104,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400DB430-A22D-402B-9293-AA41752103D1}">
-  <dimension ref="A2:E5"/>
+  <dimension ref="A2:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,6 +478,288 @@
         <v>18</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>127</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" ref="D6:D28" si="0">B6*100*C6/35+2</f>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" ref="E6:E28" si="1">ROUNDUP(D6,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>129</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5.77</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>15.188571428571429</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>130</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6.78</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>21.37142857142857</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>215</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>15.714285714285714</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>207</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>10.571428571428571</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>216</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="0"/>
+        <v>15.028571428571428</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>205</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>11.6</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>301</v>
+      </c>
+      <c r="B21" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="0"/>
+        <v>17.314285714285717</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D22" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D23" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D24" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D27" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D28" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Agrega espesor piso 1
</commit_message>
<xml_diff>
--- a/Tarea 02/Espesores losas.xlsx
+++ b/Tarea 02/Espesores losas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Google Drive\Trabajos\Proyecto de Hormigón Armado\proyecto-CI5206\Tarea 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{776EBD55-6951-4FEF-AC4F-7B17FD5359B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2D9361F6-7B96-45A0-A94D-D87051817E51}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{64A3EC0E-03C2-45A2-90E2-B3D1165799B2}"/>
   </bookViews>
@@ -425,7 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400DB430-A22D-402B-9293-AA41752103D1}">
   <dimension ref="A2:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Agregue tablas de losas y vigas para informe
</commit_message>
<xml_diff>
--- a/Tarea 02/Espesores losas.xlsx
+++ b/Tarea 02/Espesores losas.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Google Drive\Trabajos\Proyecto de Hormigón Armado\proyecto-CI5206\Tarea 02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Google Drive\proyecto de hormigon\proyecto-CI5206\Tarea 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2D9361F6-7B96-45A0-A94D-D87051817E51}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4DC073-AE94-4CE4-BA0E-40982EBD4576}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{64A3EC0E-03C2-45A2-90E2-B3D1165799B2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="1" xr2:uid="{64A3EC0E-03C2-45A2-90E2-B3D1165799B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
   <si>
     <t>Losa</t>
   </si>
@@ -43,6 +49,99 @@
   </si>
   <si>
     <t>Techo</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>tipo 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tipo 04 </t>
+  </si>
+  <si>
+    <t>tipo 10</t>
+  </si>
+  <si>
+    <t>terraza</t>
+  </si>
+  <si>
+    <t>TE01</t>
+  </si>
+  <si>
+    <t>TE02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cubierta </t>
+  </si>
+  <si>
+    <t>CU01</t>
+  </si>
+  <si>
+    <t>Piso 1</t>
+  </si>
+  <si>
+    <t>Piso 2</t>
+  </si>
+  <si>
+    <t>Piso 3</t>
+  </si>
+  <si>
+    <t>Piso tipo</t>
+  </si>
+  <si>
+    <t>Piso 24</t>
+  </si>
+  <si>
+    <t>Techumbre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cubierta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piso 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piso 3 </t>
+  </si>
+  <si>
+    <t>Piso Tipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Techumbre </t>
+  </si>
+  <si>
+    <t>Cubierta</t>
+  </si>
+  <si>
+    <t>Espesor (cm)</t>
+  </si>
+  <si>
+    <t>e (cm)</t>
+  </si>
+  <si>
+    <t>e red (cm)</t>
+  </si>
+  <si>
+    <t>Largo critico (m)</t>
+  </si>
+  <si>
+    <t>Apoyos</t>
+  </si>
+  <si>
+    <t>Empotrado - Apoyado</t>
+  </si>
+  <si>
+    <t>Empotrado - Empotrado</t>
+  </si>
+  <si>
+    <t>Apoyado - Apoyado</t>
+  </si>
+  <si>
+    <t>Altura máxima [cm]</t>
+  </si>
+  <si>
+    <t>Largo máximo [m]</t>
   </si>
 </sst>
 </file>
@@ -80,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -88,11 +187,215 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -108,6 +411,123 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400DB430-A22D-402B-9293-AA41752103D1}">
-  <dimension ref="A2:E28"/>
+  <dimension ref="A2:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,7 +909,7 @@
         <v>0.6</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" ref="D6:D28" si="0">B6*100*C6/35+2</f>
+        <f t="shared" ref="D6:D23" si="0">B6*100*C6/35+2</f>
         <v>16.399999999999999</v>
       </c>
       <c r="E6" s="1">
@@ -676,92 +1096,919 @@
         <v>301</v>
       </c>
       <c r="B21" s="1">
-        <v>6.7</v>
+        <v>5.95</v>
       </c>
       <c r="C21" s="1">
         <v>0.8</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="0"/>
-        <v>17.314285714285717</v>
+        <v>15.6</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>304</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5.95</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.8</v>
+      </c>
       <c r="D22" s="4">
         <f t="shared" si="0"/>
+        <v>15.6</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>305</v>
+      </c>
+      <c r="B23" s="1">
+        <v>7.16</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="0"/>
+        <v>14.274285714285714</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="1">
-        <f t="shared" si="1"/>
+      <c r="D27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1">
+        <v>6.01</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" ref="D28:D30" si="2">B28*100*C28/35+2</f>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" ref="E28:E30" si="3">ROUNDUP(D28,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6.01</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="2"/>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="1">
+        <v>5.62</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="2"/>
+        <v>14.845714285714287</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D23" s="4">
-        <f t="shared" si="0"/>
+      <c r="D34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>2401</v>
+      </c>
+      <c r="B35" s="1">
+        <v>6.01</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" ref="D35:D37" si="4">B35*100*C35/35+2</f>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" ref="E35:E37" si="5">ROUNDUP(D35,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>2404</v>
+      </c>
+      <c r="B36" s="1">
+        <v>6.01</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="4"/>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>2405</v>
+      </c>
+      <c r="B37" s="1">
+        <v>5.62</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="4"/>
+        <v>14.845714285714287</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="1">
-        <f t="shared" si="1"/>
+      <c r="D41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" ref="D42" si="6">B42*100*C42/35+2</f>
+        <v>6.628571428571429</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" ref="E42" si="7">ROUNDUP(D42,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" ref="D43" si="8">B43*100*C43/35+2</f>
+        <v>8</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" ref="E43" si="9">ROUNDUP(D43,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D44" s="4"/>
+    </row>
+    <row r="46" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D24" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E24" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D25" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E25" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D26" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E26" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D27" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E27" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D28" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E28" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
+      <c r="D48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" ref="D49" si="10">B49*100*C49/35+2</f>
+        <v>5.2571428571428571</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" ref="E49" si="11">ROUNDUP(D49,0)</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A33214-E392-40E8-BD38-0F3A6A253B89}">
+  <dimension ref="B2:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6">
+        <v>110</v>
+      </c>
+      <c r="D4" s="7">
+        <v>5.56</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <f>D4*100*E4/35+2</f>
+        <v>17.885714285714286</v>
+      </c>
+      <c r="G4" s="9">
+        <f>ROUNDUP(F4,0)</f>
+        <v>18</v>
+      </c>
+      <c r="I4" s="41">
+        <v>50</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="30">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="20"/>
+      <c r="C5" s="10">
+        <v>127</v>
+      </c>
+      <c r="D5" s="11">
+        <v>8.4</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" ref="F5:F23" si="0">D5*100*E5/35+2</f>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" ref="G5:G23" si="1">ROUNDUP(F5,0)</f>
+        <v>17</v>
+      </c>
+      <c r="I5" s="38"/>
+      <c r="J5" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="20"/>
+      <c r="C6" s="10">
+        <v>129</v>
+      </c>
+      <c r="D6" s="11">
+        <v>5.77</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="0"/>
+        <v>15.188571428571429</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I6" s="42"/>
+      <c r="J6" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="44">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="21"/>
+      <c r="C7" s="14">
+        <v>130</v>
+      </c>
+      <c r="D7" s="15">
+        <v>6.78</v>
+      </c>
+      <c r="E7" s="15">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16">
+        <f t="shared" si="0"/>
+        <v>21.37142857142857</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I7" s="38">
+        <v>30</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="31">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="6">
+        <v>215</v>
+      </c>
+      <c r="D8" s="7">
+        <v>6</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>15.714285714285714</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I8" s="38"/>
+      <c r="J8" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="20"/>
+      <c r="C9" s="10">
+        <v>207</v>
+      </c>
+      <c r="D9" s="11">
+        <v>5</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="0"/>
+        <v>10.571428571428571</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I9" s="39"/>
+      <c r="J9" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="20"/>
+      <c r="C10" s="10">
+        <v>216</v>
+      </c>
+      <c r="D10" s="11">
+        <v>5.7</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="0"/>
+        <v>15.028571428571428</v>
+      </c>
+      <c r="G10" s="13">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="21"/>
+      <c r="C11" s="14">
+        <v>205</v>
+      </c>
+      <c r="D11" s="15">
+        <v>5.6</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" si="0"/>
+        <v>11.6</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6">
+        <v>301</v>
+      </c>
+      <c r="D12" s="7">
+        <v>5.95</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>15.6</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="20"/>
+      <c r="C13" s="10">
+        <v>304</v>
+      </c>
+      <c r="D13" s="11">
+        <v>5.95</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="0"/>
+        <v>15.6</v>
+      </c>
+      <c r="G13" s="13">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="21"/>
+      <c r="C14" s="14">
+        <v>305</v>
+      </c>
+      <c r="D14" s="15">
+        <v>7.16</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F14" s="16">
+        <f t="shared" si="0"/>
+        <v>14.274285714285714</v>
+      </c>
+      <c r="G14" s="17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="7">
+        <v>6.01</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="20"/>
+      <c r="C16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="11">
+        <v>6.01</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="0"/>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="G16" s="13">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="21"/>
+      <c r="C17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="15">
+        <v>5.62</v>
+      </c>
+      <c r="E17" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="16">
+        <f t="shared" si="0"/>
+        <v>14.845714285714287</v>
+      </c>
+      <c r="G17" s="17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2401</v>
+      </c>
+      <c r="D18" s="7">
+        <v>6.01</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="20"/>
+      <c r="C19" s="10">
+        <v>2404</v>
+      </c>
+      <c r="D19" s="11">
+        <v>6.01</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="0"/>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="G19" s="13">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="21"/>
+      <c r="C20" s="14">
+        <v>2405</v>
+      </c>
+      <c r="D20" s="15">
+        <v>5.62</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="F20" s="16">
+        <f t="shared" si="0"/>
+        <v>14.845714285714287</v>
+      </c>
+      <c r="G20" s="17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="F21" s="8">
+        <f t="shared" si="0"/>
+        <v>6.628571428571429</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="21"/>
+      <c r="C22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="E22" s="15">
+        <v>1</v>
+      </c>
+      <c r="F22" s="16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G22" s="17">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="26">
+        <v>1.9</v>
+      </c>
+      <c r="E23" s="26">
+        <v>0.6</v>
+      </c>
+      <c r="F23" s="27">
+        <f t="shared" si="0"/>
+        <v>5.2571428571428571</v>
+      </c>
+      <c r="G23" s="24">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="18"/>
+      <c r="C25" s="36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="32">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
corregimos espesor de losa piso 1 por condicion de empotramiento
</commit_message>
<xml_diff>
--- a/Tarea 02/Espesores losas.xlsx
+++ b/Tarea 02/Espesores losas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Google Drive\proyecto de hormigon\proyecto-CI5206\Tarea 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4DC073-AE94-4CE4-BA0E-40982EBD4576}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9B936C-946A-434E-948B-4ECF369F3015}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="1" xr2:uid="{64A3EC0E-03C2-45A2-90E2-B3D1165799B2}"/>
   </bookViews>
@@ -451,6 +451,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -460,37 +484,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -502,32 +520,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400DB430-A22D-402B-9293-AA41752103D1}">
   <dimension ref="A2:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:E49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,15 +887,15 @@
         <v>5.56</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D5" s="4">
         <f>B5*100*C5/35+2</f>
-        <v>17.885714285714286</v>
+        <v>11.53142857142857</v>
       </c>
       <c r="E5" s="1">
         <f>ROUNDUP(D5,0)</f>
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -913,7 +913,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" ref="E6:E28" si="1">ROUNDUP(D6,0)</f>
+        <f t="shared" ref="E6:E23" si="1">ROUNDUP(D6,0)</f>
         <v>17</v>
       </c>
     </row>
@@ -944,15 +944,15 @@
         <v>6.78</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>21.37142857142857</v>
+        <v>13.622857142857143</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1433,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A33214-E392-40E8-BD38-0F3A6A253B89}">
-  <dimension ref="B2:K32"/>
+  <dimension ref="B2:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:C32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="B24:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1449,65 +1449,65 @@
   <sheetData>
     <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>110</v>
       </c>
       <c r="D4" s="7">
         <v>5.56</v>
       </c>
       <c r="E4" s="7">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="F4" s="8">
         <f>D4*100*E4/35+2</f>
-        <v>17.885714285714286</v>
+        <v>11.53142857142857</v>
       </c>
       <c r="G4" s="9">
         <f>ROUNDUP(F4,0)</f>
-        <v>18</v>
-      </c>
-      <c r="I4" s="41">
+        <v>12</v>
+      </c>
+      <c r="I4" s="35">
         <v>50</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="30">
+      <c r="K4" s="24">
         <v>7.5</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="20"/>
-      <c r="C5" s="10">
+      <c r="B5" s="40"/>
+      <c r="C5" s="11">
         <v>127</v>
       </c>
       <c r="D5" s="11">
@@ -1517,496 +1517,476 @@
         <v>0.6</v>
       </c>
       <c r="F5" s="12">
-        <f t="shared" ref="F5:F23" si="0">D5*100*E5/35+2</f>
+        <f t="shared" ref="F5" si="0">D5*100*E5/35+2</f>
         <v>16.399999999999999</v>
       </c>
       <c r="G5" s="13">
-        <f t="shared" ref="G5:G23" si="1">ROUNDUP(F5,0)</f>
+        <f t="shared" ref="G5" si="1">ROUNDUP(F5,0)</f>
         <v>17</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="34" t="s">
+      <c r="I5" s="36"/>
+      <c r="J5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="25">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="10">
-        <v>129</v>
-      </c>
-      <c r="D6" s="11">
-        <v>5.77</v>
-      </c>
-      <c r="E6" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="F6" s="12">
-        <f t="shared" si="0"/>
-        <v>15.188571428571429</v>
-      </c>
-      <c r="G6" s="13">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="I6" s="42"/>
-      <c r="J6" s="43" t="s">
+    <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="41"/>
+      <c r="C6" s="15">
+        <v>130</v>
+      </c>
+      <c r="D6" s="15">
+        <v>6.78</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F6" s="16">
+        <f t="shared" ref="F4:F6" si="2">D6*100*E6/35+2</f>
+        <v>13.622857142857143</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" ref="G4:G6" si="3">ROUNDUP(F6,0)</f>
+        <v>14</v>
+      </c>
+      <c r="I6" s="37"/>
+      <c r="J6" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="44">
+      <c r="K6" s="34">
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="21"/>
-      <c r="C7" s="14">
-        <v>130</v>
-      </c>
-      <c r="D7" s="15">
-        <v>6.78</v>
-      </c>
-      <c r="E7" s="15">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6">
+        <v>215</v>
+      </c>
+      <c r="D7" s="7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" ref="F7:F22" si="4">D7*100*E7/35+2</f>
+        <v>15.714285714285714</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" ref="G7:G22" si="5">ROUNDUP(F7,0)</f>
+        <v>16</v>
+      </c>
+      <c r="I7" s="36">
+        <v>30</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="25">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="40"/>
+      <c r="C8" s="10">
+        <v>207</v>
+      </c>
+      <c r="D8" s="11">
+        <v>5</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="4"/>
+        <v>10.571428571428571</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="I8" s="36"/>
+      <c r="J8" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="40"/>
+      <c r="C9" s="10">
+        <v>216</v>
+      </c>
+      <c r="D9" s="11">
+        <v>5.7</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="4"/>
+        <v>15.028571428571428</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="I9" s="38"/>
+      <c r="J9" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="26">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="41"/>
+      <c r="C10" s="14">
+        <v>205</v>
+      </c>
+      <c r="D10" s="15">
+        <v>5.6</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="16">
+        <f t="shared" si="4"/>
+        <v>11.6</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6">
+        <v>301</v>
+      </c>
+      <c r="D11" s="7">
+        <v>5.95</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="4"/>
+        <v>15.6</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="40"/>
+      <c r="C12" s="10">
+        <v>304</v>
+      </c>
+      <c r="D12" s="11">
+        <v>5.95</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="4"/>
+        <v>15.6</v>
+      </c>
+      <c r="G12" s="13">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="41"/>
+      <c r="C13" s="14">
+        <v>305</v>
+      </c>
+      <c r="D13" s="15">
+        <v>7.16</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F13" s="16">
+        <f t="shared" si="4"/>
+        <v>14.274285714285714</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="7">
+        <v>6.01</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="4"/>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="40"/>
+      <c r="C15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="11">
+        <v>6.01</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="4"/>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="G15" s="13">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="41"/>
+      <c r="C16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="15">
+        <v>5.62</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="F16" s="16">
+        <f t="shared" si="4"/>
+        <v>14.845714285714287</v>
+      </c>
+      <c r="G16" s="17">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2401</v>
+      </c>
+      <c r="D17" s="7">
+        <v>6.01</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="4"/>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="40"/>
+      <c r="C18" s="10">
+        <v>2404</v>
+      </c>
+      <c r="D18" s="11">
+        <v>6.01</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="4"/>
+        <v>15.737142857142857</v>
+      </c>
+      <c r="G18" s="13">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="41"/>
+      <c r="C19" s="14">
+        <v>2405</v>
+      </c>
+      <c r="D19" s="15">
+        <v>5.62</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="F19" s="16">
+        <f t="shared" si="4"/>
+        <v>14.845714285714287</v>
+      </c>
+      <c r="G19" s="17">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="4"/>
+        <v>6.628571428571429</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="41"/>
+      <c r="C21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="E21" s="15">
         <v>1</v>
       </c>
-      <c r="F7" s="16">
-        <f t="shared" si="0"/>
-        <v>21.37142857142857</v>
-      </c>
-      <c r="G7" s="17">
-        <f t="shared" si="1"/>
+      <c r="F21" s="16">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G21" s="17">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="21">
+        <v>1.9</v>
+      </c>
+      <c r="E22" s="21">
+        <v>0.6</v>
+      </c>
+      <c r="F22" s="22">
+        <f t="shared" si="4"/>
+        <v>5.2571428571428571</v>
+      </c>
+      <c r="G22" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="18"/>
+      <c r="C24" s="30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="24">
+        <f>MAX(G4:G6)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="38">
-        <v>30</v>
-      </c>
-      <c r="J7" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="31">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="6">
-        <v>215</v>
-      </c>
-      <c r="D8" s="7">
-        <v>6</v>
-      </c>
-      <c r="E8" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="F8" s="8">
-        <f t="shared" si="0"/>
-        <v>15.714285714285714</v>
-      </c>
-      <c r="G8" s="9">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="20"/>
-      <c r="C9" s="10">
-        <v>207</v>
-      </c>
-      <c r="D9" s="11">
-        <v>5</v>
-      </c>
-      <c r="E9" s="11">
-        <v>0.6</v>
-      </c>
-      <c r="F9" s="12">
-        <f t="shared" si="0"/>
-        <v>10.571428571428571</v>
-      </c>
-      <c r="G9" s="13">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="I9" s="39"/>
-      <c r="J9" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" s="32">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="20"/>
-      <c r="C10" s="10">
-        <v>216</v>
-      </c>
-      <c r="D10" s="11">
-        <v>5.7</v>
-      </c>
-      <c r="E10" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="F10" s="12">
-        <f t="shared" si="0"/>
-        <v>15.028571428571428</v>
-      </c>
-      <c r="G10" s="13">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="21"/>
-      <c r="C11" s="14">
-        <v>205</v>
-      </c>
-      <c r="D11" s="15">
-        <v>5.6</v>
-      </c>
-      <c r="E11" s="15">
-        <v>0.6</v>
-      </c>
-      <c r="F11" s="16">
-        <f t="shared" si="0"/>
-        <v>11.6</v>
-      </c>
-      <c r="G11" s="17">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="6">
-        <v>301</v>
-      </c>
-      <c r="D12" s="7">
-        <v>5.95</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="F12" s="8">
-        <f t="shared" si="0"/>
-        <v>15.6</v>
-      </c>
-      <c r="G12" s="9">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="20"/>
-      <c r="C13" s="10">
-        <v>304</v>
-      </c>
-      <c r="D13" s="11">
-        <v>5.95</v>
-      </c>
-      <c r="E13" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="F13" s="12">
-        <f t="shared" si="0"/>
-        <v>15.6</v>
-      </c>
-      <c r="G13" s="13">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="21"/>
-      <c r="C14" s="14">
-        <v>305</v>
-      </c>
-      <c r="D14" s="15">
-        <v>7.16</v>
-      </c>
-      <c r="E14" s="15">
-        <v>0.6</v>
-      </c>
-      <c r="F14" s="16">
-        <f t="shared" si="0"/>
-        <v>14.274285714285714</v>
-      </c>
-      <c r="G14" s="17">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="7">
-        <v>6.01</v>
-      </c>
-      <c r="E15" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="F15" s="8">
-        <f t="shared" si="0"/>
-        <v>15.737142857142857</v>
-      </c>
-      <c r="G15" s="9">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="20"/>
-      <c r="C16" s="10" t="s">
+      <c r="C26" s="25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="25">
         <v>8</v>
       </c>
-      <c r="D16" s="11">
-        <v>6.01</v>
-      </c>
-      <c r="E16" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="F16" s="12">
-        <f t="shared" si="0"/>
-        <v>15.737142857142857</v>
-      </c>
-      <c r="G16" s="13">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="21"/>
-      <c r="C17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="15">
-        <v>5.62</v>
-      </c>
-      <c r="E17" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="F17" s="16">
-        <f t="shared" si="0"/>
-        <v>14.845714285714287</v>
-      </c>
-      <c r="G17" s="17">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="6">
-        <v>2401</v>
-      </c>
-      <c r="D18" s="7">
-        <v>6.01</v>
-      </c>
-      <c r="E18" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="F18" s="8">
-        <f t="shared" si="0"/>
-        <v>15.737142857142857</v>
-      </c>
-      <c r="G18" s="9">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="20"/>
-      <c r="C19" s="10">
-        <v>2404</v>
-      </c>
-      <c r="D19" s="11">
-        <v>6.01</v>
-      </c>
-      <c r="E19" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="F19" s="12">
-        <f t="shared" si="0"/>
-        <v>15.737142857142857</v>
-      </c>
-      <c r="G19" s="13">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="21"/>
-      <c r="C20" s="14">
-        <v>2405</v>
-      </c>
-      <c r="D20" s="15">
-        <v>5.62</v>
-      </c>
-      <c r="E20" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="F20" s="16">
-        <f t="shared" si="0"/>
-        <v>14.845714285714287</v>
-      </c>
-      <c r="G20" s="17">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="19" t="s">
+    </row>
+    <row r="31" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="26">
         <v>20</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="7">
-        <v>2.7</v>
-      </c>
-      <c r="E21" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="F21" s="8">
-        <f t="shared" si="0"/>
-        <v>6.628571428571429</v>
-      </c>
-      <c r="G21" s="9">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="21"/>
-      <c r="C22" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="15">
-        <v>2.1</v>
-      </c>
-      <c r="E22" s="15">
-        <v>1</v>
-      </c>
-      <c r="F22" s="16">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G22" s="17">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="26">
-        <v>1.9</v>
-      </c>
-      <c r="E23" s="26">
-        <v>0.6</v>
-      </c>
-      <c r="F23" s="27">
-        <f t="shared" si="0"/>
-        <v>5.2571428571428571</v>
-      </c>
-      <c r="G23" s="24">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="18"/>
-      <c r="C25" s="36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="30">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="31">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="31">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="31">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="31">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="31">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="32">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="I4:I6"/>
     <mergeCell ref="I7:I9"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>